<commit_message>
hex, hex logic, register init
</commit_message>
<xml_diff>
--- a/Next State Table.xlsx
+++ b/Next State Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neilr\Desktop\Project_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A79C95D2-CEFA-4F4A-AD31-D18544FF6755}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99354809-3716-4599-981C-068542D45811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="2790" windowWidth="29040" windowHeight="15840" xr2:uid="{2B082B8A-6F23-42B4-86A6-F5AB09BE1258}"/>
+    <workbookView xWindow="38280" yWindow="2745" windowWidth="29040" windowHeight="15840" xr2:uid="{2B082B8A-6F23-42B4-86A6-F5AB09BE1258}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -545,7 +545,7 @@
   <dimension ref="A1:U60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -792,7 +792,7 @@
         <v>0</v>
       </c>
       <c r="I5" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5" s="9" t="s">
         <v>5</v>

</xml_diff>